<commit_message>
working on potential matlab code for array analysis
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahbook/Box Sync/projects/biobank/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F3605B-1396-E545-9AA2-53E45CD9B02D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99044626-3265-B646-8EA6-401105B5D876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16640" yWindow="-18340" windowWidth="12800" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
@@ -1062,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
trying to fix online analysis
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -1,34 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahbook/Box Sync/projects/biobank/raw_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Documents\GitHub\biobank\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99044626-3265-B646-8EA6-401105B5D876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B0D383-0FDE-4985-AE07-FFB30BA8A572}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
   <si>
     <t>ID</t>
   </si>
@@ -208,6 +200,21 @@
   </si>
   <si>
     <t>merged files without issue</t>
+  </si>
+  <si>
+    <t>Marginal</t>
+  </si>
+  <si>
+    <t>LCX</t>
+  </si>
+  <si>
+    <t>Time_Stent_4</t>
+  </si>
+  <si>
+    <t>Location_Stent_4</t>
+  </si>
+  <si>
+    <t>Unknown</t>
   </si>
 </sst>
 </file>
@@ -1060,34 +1067,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" customWidth="1"/>
-    <col min="14" max="14" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" customWidth="1"/>
-    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="4" max="4" width="19.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="15.125" customWidth="1"/>
+    <col min="12" max="12" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.125" customWidth="1"/>
+    <col min="14" max="14" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" customWidth="1"/>
+    <col min="16" max="16" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.125" customWidth="1"/>
+    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1122,25 +1129,31 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1155,7 +1168,7 @@
         <v>0.63750000000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -1170,7 +1183,7 @@
         <v>0.48541666666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -1183,8 +1196,53 @@
       <c r="D4" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.74236111111111114</v>
+      </c>
+      <c r="I4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.74513888888888891</v>
+      </c>
+      <c r="K4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.75624999999999998</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="O4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.69305555555555554</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" s="2">
+        <v>0.70694444444444438</v>
+      </c>
+      <c r="S4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1196,7 +1254,7 @@
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1208,7 +1266,7 @@
       </c>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -1220,7 +1278,7 @@
       </c>
       <c r="D7" s="6"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
@@ -1232,7 +1290,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -1243,7 +1301,7 @@
         <v>0.52361111111111114</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -1257,7 +1315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1268,7 +1326,7 @@
         <v>0.38541666666666669</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -1279,7 +1337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -1290,7 +1348,7 @@
         <v>0.49374999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
@@ -1304,7 +1362,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>44</v>
       </c>
@@ -1315,7 +1373,7 @@
         <v>0.50972222222222219</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -1326,7 +1384,7 @@
         <v>0.5229166666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -1337,7 +1395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
@@ -1348,7 +1406,7 @@
         <v>0.41597222222222219</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1359,7 +1417,7 @@
         <v>0.48819444444444443</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
@@ -1370,7 +1428,7 @@
         <v>0.44027777777777777</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1381,7 +1439,7 @@
         <v>0.34722222222222227</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
pilot data being worked on, also updated cluster to just handle new data
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Documents\GitHub\biobank\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B0D383-0FDE-4985-AE07-FFB30BA8A572}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4E1E3A-E134-486B-8BFC-FC01BB7D72B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="468" windowWidth="25608" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>ID</t>
   </si>
@@ -37,42 +37,6 @@
     <t>Time_LHC</t>
   </si>
   <si>
-    <t>Time_Stent_1</t>
-  </si>
-  <si>
-    <t>Location_Stent_1</t>
-  </si>
-  <si>
-    <t>Time_Stent_2</t>
-  </si>
-  <si>
-    <t>Location_Stent_2</t>
-  </si>
-  <si>
-    <t>Time_Stent_3</t>
-  </si>
-  <si>
-    <t>Location_Stent_3</t>
-  </si>
-  <si>
-    <t>Time_Balloon_1</t>
-  </si>
-  <si>
-    <t>Location_Balloon_1</t>
-  </si>
-  <si>
-    <t>Time_Balloon_2</t>
-  </si>
-  <si>
-    <t>Location_Balloon_2</t>
-  </si>
-  <si>
-    <t>Time_Balloon_3</t>
-  </si>
-  <si>
-    <t>Location_Balloon_23</t>
-  </si>
-  <si>
     <t>06925</t>
   </si>
   <si>
@@ -202,19 +166,43 @@
     <t>merged files without issue</t>
   </si>
   <si>
-    <t>Marginal</t>
-  </si>
-  <si>
-    <t>LCX</t>
-  </si>
-  <si>
-    <t>Time_Stent_4</t>
-  </si>
-  <si>
-    <t>Location_Stent_4</t>
-  </si>
-  <si>
-    <t>Unknown</t>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>processed</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>07027</t>
+  </si>
+  <si>
+    <t>07032</t>
+  </si>
+  <si>
+    <t>07036</t>
+  </si>
+  <si>
+    <t>07037</t>
+  </si>
+  <si>
+    <t>07045</t>
+  </si>
+  <si>
+    <t>07052</t>
+  </si>
+  <si>
+    <t>07053</t>
+  </si>
+  <si>
+    <t>07063</t>
+  </si>
+  <si>
+    <t>07071</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -1067,34 +1055,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.125" customWidth="1"/>
-    <col min="4" max="4" width="19.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="15.125" customWidth="1"/>
-    <col min="12" max="12" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.125" customWidth="1"/>
-    <col min="14" max="14" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.125" customWidth="1"/>
-    <col min="16" max="16" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.125" customWidth="1"/>
-    <col min="18" max="18" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.09765625" customWidth="1"/>
+    <col min="4" max="4" width="19.09765625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,54 +1088,15 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>0.55833333333333335</v>
@@ -1167,13 +1105,16 @@
       <c r="E2" s="2">
         <v>0.63750000000000007</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>0.43541666666666662</v>
@@ -1182,272 +1123,362 @@
       <c r="E3" s="2">
         <v>0.48541666666666666</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2">
         <v>0.45</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2">
         <v>0.65833333333333333</v>
       </c>
-      <c r="F4" s="2">
-        <v>0.71597222222222223</v>
-      </c>
-      <c r="G4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0.74236111111111114</v>
-      </c>
-      <c r="I4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.74513888888888891</v>
-      </c>
-      <c r="K4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0.75624999999999998</v>
-      </c>
-      <c r="M4" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.68472222222222223</v>
-      </c>
-      <c r="O4" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.69305555555555554</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" s="2">
-        <v>0.70694444444444438</v>
-      </c>
-      <c r="S4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2">
         <v>0.41111111111111115</v>
       </c>
       <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2">
         <v>0.47638888888888892</v>
       </c>
       <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3">
         <v>0.5083333333333333</v>
       </c>
       <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2">
         <v>0.52361111111111114</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C10" s="2">
         <v>0.44791666666666669</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C11" s="2">
         <v>0.38541666666666669</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2">
         <v>0.49374999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2">
         <v>0.51041666666666663</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2">
         <v>0.50972222222222219</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C16" s="2">
         <v>0.5229166666666667</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C18" s="2">
         <v>0.41597222222222219</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2">
         <v>0.48819444444444443</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C20" s="2">
         <v>0.44027777777777777</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2">
         <v>0.34722222222222227</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C22" s="2">
         <v>0.68611111111111101</v>
+      </c>
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected depression and reanalyzing it
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4E1E3A-E134-486B-8BFC-FC01BB7D72B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4E1E3A-E134-486B-8BFC-FC01BB7D72B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="468" windowWidth="25608" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -37,12 +45,18 @@
     <t>Time_LHC</t>
   </si>
   <si>
+    <t>Status</t>
+  </si>
+  <si>
     <t>06925</t>
   </si>
   <si>
     <t>08/05/2019</t>
   </si>
   <si>
+    <t>processed</t>
+  </si>
+  <si>
     <t>06928</t>
   </si>
   <si>
@@ -97,6 +111,12 @@
     <t>09/04/2019</t>
   </si>
   <si>
+    <t>file initially listed as part 1, data is only 137k, archiving this</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
     <t>06977</t>
   </si>
   <si>
@@ -118,6 +138,9 @@
     <t>06984</t>
   </si>
   <si>
+    <t>merged files without issue</t>
+  </si>
+  <si>
     <t>06988</t>
   </si>
   <si>
@@ -160,43 +183,46 @@
     <t>07014</t>
   </si>
   <si>
-    <t>file initially listed as part 1, data is only 137k, archiving this</t>
-  </si>
-  <si>
-    <t>merged files without issue</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>processed</t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>07027</t>
   </si>
   <si>
+    <t>10/14/2019</t>
+  </si>
+  <si>
     <t>07032</t>
   </si>
   <si>
+    <t>10/17/2019</t>
+  </si>
+  <si>
     <t>07036</t>
   </si>
   <si>
+    <t>10/21/2019</t>
+  </si>
+  <si>
     <t>07037</t>
   </si>
   <si>
     <t>07045</t>
   </si>
   <si>
+    <t>10/24/2019</t>
+  </si>
+  <si>
     <t>07052</t>
   </si>
   <si>
+    <t>10/30/2019</t>
+  </si>
+  <si>
     <t>07053</t>
   </si>
   <si>
     <t>07063</t>
+  </si>
+  <si>
+    <t>11/11/2019</t>
   </si>
   <si>
     <t>07071</t>
@@ -209,7 +235,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1059,19 +1085,19 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A32" sqref="A32"/>
+      <selection pane="topRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.09765625" customWidth="1"/>
-    <col min="4" max="4" width="19.09765625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
+    <col min="4" max="4" width="19.125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1088,15 +1114,15 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>0.55833333333333335</v>
@@ -1106,15 +1132,15 @@
         <v>0.63750000000000007</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2">
         <v>0.43541666666666662</v>
@@ -1124,361 +1150,454 @@
         <v>0.48541666666666666</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="46.9">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>0.45</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
         <v>0.65833333333333333</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2">
         <v>0.41111111111111115</v>
       </c>
       <c r="D5" s="5"/>
       <c r="F5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>0.47638888888888892</v>
       </c>
       <c r="D6" s="5"/>
+      <c r="E6" s="2">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="3">
         <v>0.5083333333333333</v>
       </c>
       <c r="D7" s="6"/>
+      <c r="E7" s="2">
+        <v>0.61319444444444449</v>
+      </c>
       <c r="F7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5"/>
+      <c r="E8" s="2">
+        <v>0.46388888888888885</v>
+      </c>
       <c r="F8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" s="2">
         <v>0.52361111111111114</v>
       </c>
+      <c r="E9" s="2">
+        <v>0.39652777777777781</v>
+      </c>
       <c r="F9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="46.8" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="46.9">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2">
         <v>0.44791666666666669</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.64861111111111114</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C11" s="2">
         <v>0.38541666666666669</v>
       </c>
+      <c r="E11" s="2">
+        <v>0.41250000000000003</v>
+      </c>
       <c r="F11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>32</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.44375000000000003</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C13" s="2">
         <v>0.49374999999999997</v>
       </c>
+      <c r="E13" s="2">
+        <v>0.53888888888888886</v>
+      </c>
       <c r="F13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="31.15">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2">
         <v>0.51041666666666663</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.57500000000000007</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C15" s="2">
         <v>0.50972222222222219</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C16" s="2">
         <v>0.5229166666666667</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2">
         <v>0.41597222222222219</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C19" s="2">
         <v>0.48819444444444443</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2">
         <v>0.44027777777777777</v>
       </c>
       <c r="F20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C21" s="2">
         <v>0.34722222222222227</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2">
         <v>0.68611111111111101</v>
       </c>
       <c r="F22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.43611111111111112</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.73055555555555562</v>
+      </c>
       <c r="F23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.49513888888888885</v>
       </c>
       <c r="F24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.4680555555555555</v>
       </c>
       <c r="F25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.58124999999999993</v>
       </c>
       <c r="F26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.39652777777777781</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.53263888888888888</v>
       </c>
       <c r="F27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.47083333333333338</v>
       </c>
       <c r="F28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.51388888888888895</v>
       </c>
       <c r="F29" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.48680555555555555</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on presentation for METRIC RIP presentation
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4E1E3A-E134-486B-8BFC-FC01BB7D72B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90E1A6F-3E4E-4A04-AD52-1CDF7AB2BFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="25608" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -228,14 +228,14 @@
     <t>07071</t>
   </si>
   <si>
-    <t>new</t>
+    <t>haven't analyzed yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1083,12 +1083,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B4" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
@@ -1097,7 +1097,7 @@
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="46.9">
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="46.9">
+    <row r="10" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.15">
+    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1601,12 +1601,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="D31" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
team project baic analysis
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,12 +15,14 @@
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>ID</t>
   </si>
@@ -229,13 +231,19 @@
   </si>
   <si>
     <t>haven't analyzed yet</t>
+  </si>
+  <si>
+    <t>07104</t>
+  </si>
+  <si>
+    <t>Patient file split in two</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1081,14 +1089,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D31" sqref="D31"/>
+      <pane xSplit="1" topLeftCell="B20" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
@@ -1097,7 +1105,7 @@
     <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1125,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -1153,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1173,7 +1181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1206,7 +1214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1224,7 +1232,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1242,7 +1250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -1259,7 +1267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="47.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -1296,7 +1304,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -1313,7 +1321,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -1330,7 +1338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="31.5">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -1350,7 +1358,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1367,7 +1375,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -1384,7 +1392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -1401,7 +1409,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
         <v>46</v>
       </c>
@@ -1443,7 +1451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
         <v>48</v>
       </c>
@@ -1457,7 +1465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
         <v>50</v>
       </c>
@@ -1471,7 +1479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
@@ -1488,7 +1496,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>53</v>
       </c>
@@ -1505,7 +1513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
         <v>55</v>
       </c>
@@ -1519,7 +1527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>57</v>
       </c>
@@ -1533,7 +1541,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
@@ -1550,7 +1558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
         <v>60</v>
       </c>
@@ -1567,7 +1575,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
@@ -1584,7 +1592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
@@ -1601,7 +1609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
         <v>65</v>
       </c>
@@ -1610,6 +1618,14 @@
       </c>
       <c r="F31" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="31.5">
+      <c r="A32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated biobank weekly meeting of 2/11/20
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B013291B-2140-4525-BD7E-90670F6F9915}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAE259C-E6EE-442A-B9B7-5D2D53AC7E22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -257,12 +257,18 @@
     <t>07103</t>
   </si>
   <si>
+    <t>HT</t>
+  </si>
+  <si>
     <t>07104</t>
   </si>
   <si>
     <t>Patient file split in two</t>
   </si>
   <si>
+    <t>LHC</t>
+  </si>
+  <si>
     <t>07106</t>
   </si>
   <si>
@@ -275,6 +281,12 @@
     <t>01/09/2020</t>
   </si>
   <si>
+    <t>13:32:05-1:32:17 </t>
+  </si>
+  <si>
+    <t>RHC</t>
+  </si>
+  <si>
     <t>07111</t>
   </si>
   <si>
@@ -327,13 +339,22 @@
   </si>
   <si>
     <t xml:space="preserve">File split in two parts. </t>
+  </si>
+  <si>
+    <t>07143</t>
+  </si>
+  <si>
+    <t>02/05/2020</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -464,6 +485,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -810,7 +838,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -824,6 +852,10 @@
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1179,868 +1211,933 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B21" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.125" customWidth="1"/>
-    <col min="4" max="4" width="19.125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="14.58203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.08203125" customWidth="1"/>
+    <col min="5" max="5" width="19.08203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>0.55833333333333335</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="2">
+      <c r="E2" s="5"/>
+      <c r="F2" s="2">
         <v>0.63750000000000007</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>0.43541666666666662</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="2">
+      <c r="E3" s="5"/>
+      <c r="F3" s="2">
         <v>0.48541666666666666</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="46.5">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="2">
         <v>0.45</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>0.65833333333333333</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="G4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="2">
         <v>0.41111111111111115</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="E5" s="5"/>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="2">
         <v>0.47638888888888892</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2">
+      <c r="E6" s="5"/>
+      <c r="F6" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3">
+      <c r="D7" s="3">
         <v>0.5083333333333333</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="2">
+      <c r="E7" s="6"/>
+      <c r="F7" s="2">
         <v>0.61319444444444449</v>
       </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2">
+      <c r="E8" s="5"/>
+      <c r="F8" s="2">
         <v>0.46388888888888885</v>
       </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="2">
         <v>0.52361111111111114</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>0.39652777777777781</v>
       </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="46.5">
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="2">
         <v>0.44791666666666669</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="2">
         <v>0.64861111111111114</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>30</v>
       </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="2">
         <v>0.38541666666666669</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="2">
         <v>0.41250000000000003</v>
       </c>
-      <c r="F11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="2">
         <v>0.44375000000000003</v>
       </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="2">
+      <c r="D13" s="2">
         <v>0.49374999999999997</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="2">
         <v>0.53888888888888886</v>
       </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30.95">
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2">
+      <c r="D14" s="2">
         <v>0.51041666666666663</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="2">
         <v>0.57500000000000007</v>
       </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2">
+      <c r="D15" s="2">
         <v>0.50972222222222219</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="2">
         <v>0.59236111111111112</v>
       </c>
-      <c r="F15" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="2">
+      <c r="D16" s="2">
         <v>0.5229166666666667</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="2">
         <v>0.65347222222222223</v>
       </c>
-      <c r="F16" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="2">
         <v>0.50555555555555554</v>
       </c>
-      <c r="F17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="2">
+      <c r="D18" s="2">
         <v>0.41597222222222219</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="2">
         <v>0.44930555555555557</v>
       </c>
-      <c r="F18" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2">
+      <c r="D19" s="2">
         <v>0.48819444444444443</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="2">
         <v>0.54236111111111118</v>
       </c>
-      <c r="F19" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="2">
+      <c r="D20" s="2">
         <v>0.44027777777777777</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="2">
         <v>0.4777777777777778</v>
       </c>
-      <c r="F20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="2">
+      <c r="D21" s="2">
         <v>0.34722222222222227</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="2">
         <v>0.39027777777777778</v>
       </c>
-      <c r="F21" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="2">
+      <c r="D22" s="2">
         <v>0.68611111111111101</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="2">
         <v>0.64583333333333337</v>
       </c>
-      <c r="F22" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="2">
+      <c r="D23" s="2">
         <v>0.43611111111111112</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="2">
         <v>0.73055555555555562</v>
       </c>
-      <c r="F23" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="2">
+      <c r="D24" s="2">
         <v>0.39513888888888887</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="2">
         <v>0.49513888888888885</v>
       </c>
-      <c r="F24" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="2">
         <v>0.4680555555555555</v>
       </c>
-      <c r="F25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="2">
         <v>0.58124999999999993</v>
       </c>
-      <c r="F26" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="2">
+      <c r="D27" s="2">
         <v>0.39652777777777781</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="2">
         <v>0.53263888888888888</v>
       </c>
-      <c r="F27" t="s">
-        <v>10</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="2">
+      <c r="D28" s="2">
         <v>0.40069444444444446</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="2">
         <v>0.47083333333333338</v>
       </c>
-      <c r="F28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="2">
+      <c r="D29" s="2">
         <v>0.44444444444444442</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>0.51388888888888895</v>
       </c>
-      <c r="F29" t="s">
-        <v>10</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="2">
+      <c r="D30" s="2">
         <v>0.45833333333333331</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="2">
         <v>0.48680555555555555</v>
       </c>
-      <c r="F30" t="s">
-        <v>10</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C31" s="2">
+      <c r="D31" s="2">
         <v>0.4145833333333333</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="2">
         <v>0.44166666666666665</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="15.75">
+      <c r="H31" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="2">
+      <c r="D32" s="2">
         <v>0.63680555555555551</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="2">
         <v>0.6645833333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="2">
+      <c r="D33" s="2">
         <v>0.46527777777777773</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="2">
+      <c r="D34" s="2">
         <v>0.47847222222222219</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="2">
         <v>0.50486111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="2">
+      <c r="D35" s="2">
         <v>0.43333333333333335</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="2">
         <v>0.37361111111111112</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="2">
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="2">
         <v>0.50069444444444444</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="2">
         <v>0.5541666666666667</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="31.5">
+    <row r="37" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.62430555555555556</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.56111111111111112</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="H39" s="10">
+        <v>1</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="2">
-        <v>0.52777777777777779</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="2">
-        <v>0.62430555555555556</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.4145833333333333</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.4465277777777778</v>
+      </c>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="2">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.57430555555555551</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0.5395833333333333</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.59583333333333333</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C38" s="2">
-        <v>0.56111111111111112</v>
-      </c>
-      <c r="E38" s="2">
-        <v>0.6166666666666667</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="2">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E39" s="2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="2">
-        <v>0.4145833333333333</v>
-      </c>
-      <c r="E40" s="2">
-        <v>0.4465277777777778</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="1" t="s">
+      <c r="C45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0.55069444444444449</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="2">
-        <v>0.46736111111111112</v>
-      </c>
-      <c r="E41" s="2">
-        <v>0.59375</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="2">
-        <v>0.4284722222222222</v>
-      </c>
-      <c r="E42" s="2">
-        <v>0.57430555555555551</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75">
-      <c r="A43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="2">
-        <v>0.5395833333333333</v>
-      </c>
-      <c r="E43" s="2">
-        <v>0.59583333333333333</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75">
-      <c r="A44" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="2">
-        <v>0.4548611111111111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="2">
-        <v>0.55069444444444449</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="2">
-        <v>0.47222222222222227</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" s="2">
+      <c r="C47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="2">
         <v>0.60763888888888895</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="2">
+        <v>100</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D48" s="2">
         <v>0.49444444444444446</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>98</v>
+      <c r="E48" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D49" s="2">
+        <v>0.40972222222222227</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
additional patient files today, also messed up with syncing to cluster... hopefully happy recovery
</commit_message>
<xml_diff>
--- a/raw_data/patient_log.xlsx
+++ b/raw_data/patient_log.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="patient_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,11 +30,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -263,12 +266,12 @@
     <t>07104</t>
   </si>
   <si>
+    <t>LHC</t>
+  </si>
+  <si>
     <t>Patient file split in two</t>
   </si>
   <si>
-    <t>LHC</t>
-  </si>
-  <si>
     <t>07106</t>
   </si>
   <si>
@@ -278,15 +281,15 @@
     <t>07108</t>
   </si>
   <si>
+    <t>RHC</t>
+  </si>
+  <si>
     <t>01/09/2020</t>
   </si>
   <si>
     <t>13:32:05-1:32:17 </t>
   </si>
   <si>
-    <t>RHC</t>
-  </si>
-  <si>
     <t>07111</t>
   </si>
   <si>
@@ -347,14 +350,32 @@
     <t>02/05/2020</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>07152</t>
+  </si>
+  <si>
+    <t>07159</t>
+  </si>
+  <si>
+    <t>02/19/2020</t>
+  </si>
+  <si>
+    <t>07151</t>
+  </si>
+  <si>
+    <t>02/11/2020</t>
+  </si>
+  <si>
+    <t>07164</t>
+  </si>
+  <si>
+    <t>02/24/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1211,59 +1232,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A7" sqref="A7"/>
+      <pane xSplit="1" topLeftCell="B36" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.58203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.08203125" customWidth="1"/>
-    <col min="5" max="5" width="19.08203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="9.08203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="14.58203125" customWidth="1"/>
+    <col min="3" max="3" width="14.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1"/>
+    <col min="5" max="5" width="19.125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" style="10" customWidth="1"/>
+    <col min="9" max="9" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2">
         <v>0.55833333333333335</v>
@@ -1273,18 +1294,18 @@
         <v>0.63750000000000007</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2">
         <v>0.43541666666666662</v>
@@ -1294,59 +1315,59 @@
         <v>0.48541666666666666</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H3" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="46.5">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2">
         <v>0.45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2">
         <v>0.65833333333333333</v>
       </c>
       <c r="G4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H4" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2">
         <v>0.41111111111111115</v>
       </c>
       <c r="E5" s="5"/>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H5" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2">
         <v>0.47638888888888892</v>
@@ -1356,18 +1377,18 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H6" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3">
         <v>0.5083333333333333</v>
@@ -1377,39 +1398,39 @@
         <v>0.61319444444444449</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H7" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="2">
         <v>0.46388888888888885</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2">
         <v>0.52361111111111114</v>
@@ -1418,41 +1439,41 @@
         <v>0.39652777777777781</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H9" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="46.5">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2">
         <v>0.44791666666666669</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="2">
         <v>0.64861111111111114</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H10" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2">
         <v>0.38541666666666669</v>
@@ -1461,38 +1482,38 @@
         <v>0.41250000000000003</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F12" s="2">
         <v>0.44375000000000003</v>
       </c>
       <c r="G12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H12" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2">
         <v>0.49374999999999997</v>
@@ -1501,41 +1522,41 @@
         <v>0.53888888888888886</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H13" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="30.95">
       <c r="A14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D14" s="2">
         <v>0.51041666666666663</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F14" s="2">
         <v>0.57500000000000007</v>
       </c>
       <c r="G14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H14" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2">
         <v>0.50972222222222219</v>
@@ -1544,18 +1565,18 @@
         <v>0.59236111111111112</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H15" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D16" s="2">
         <v>0.5229166666666667</v>
@@ -1564,38 +1585,38 @@
         <v>0.65347222222222223</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H16" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F17" s="2">
         <v>0.50555555555555554</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2">
         <v>0.41597222222222219</v>
@@ -1604,18 +1625,18 @@
         <v>0.44930555555555557</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H18" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="D19" s="2">
         <v>0.48819444444444443</v>
@@ -1624,18 +1645,18 @@
         <v>0.54236111111111118</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H19" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" s="2">
         <v>0.44027777777777777</v>
@@ -1644,18 +1665,18 @@
         <v>0.4777777777777778</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H20" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D21" s="2">
         <v>0.34722222222222227</v>
@@ -1664,18 +1685,18 @@
         <v>0.39027777777777778</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H21" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="2">
         <v>0.68611111111111101</v>
@@ -1684,18 +1705,18 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H22" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2">
         <v>0.43611111111111112</v>
@@ -1704,18 +1725,18 @@
         <v>0.73055555555555562</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H23" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D24" s="2">
         <v>0.39513888888888887</v>
@@ -1724,52 +1745,52 @@
         <v>0.49513888888888885</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H24" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F25" s="2">
         <v>0.4680555555555555</v>
       </c>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H25" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="F26" s="2">
         <v>0.58124999999999993</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H26" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D27" s="2">
         <v>0.39652777777777781</v>
@@ -1778,18 +1799,18 @@
         <v>0.53263888888888888</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H27" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D28" s="2">
         <v>0.40069444444444446</v>
@@ -1798,18 +1819,18 @@
         <v>0.47083333333333338</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H28" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D29" s="2">
         <v>0.44444444444444442</v>
@@ -1818,18 +1839,18 @@
         <v>0.51388888888888895</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H29" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D30" s="2">
         <v>0.45833333333333331</v>
@@ -1838,35 +1859,35 @@
         <v>0.48680555555555555</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H30" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2">
         <v>0.4145833333333333</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F31" s="2">
         <v>0.44166666666666665</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H31" s="10">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" s="2">
         <v>0.63680555555555551</v>
@@ -1875,21 +1896,21 @@
         <v>0.6645833333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2">
         <v>0.46527777777777773</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D34" s="2">
         <v>0.47847222222222219</v>
@@ -1898,9 +1919,9 @@
         <v>0.50486111111111109</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D35" s="2">
         <v>0.43333333333333335</v>
@@ -1909,12 +1930,12 @@
         <v>0.37361111111111112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D36" s="2">
         <v>0.50069444444444444</v>
@@ -1923,9 +1944,9 @@
         <v>0.5541666666666667</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="31" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="30.95">
       <c r="A37" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
         <v>78</v>
@@ -1934,21 +1955,21 @@
         <v>0.52777777777777779</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F37" s="2">
         <v>0.62430555555555556</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B38" t="s">
         <v>78</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D38" s="2">
         <v>0.56111111111111112</v>
@@ -1957,15 +1978,15 @@
         <v>0.6166666666666667</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="D39" s="2">
         <v>0.52083333333333337</v>
@@ -1977,18 +1998,18 @@
         <v>1</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="2">
         <v>0.4145833333333333</v>
@@ -1998,15 +2019,15 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D41" s="2">
         <v>0.46736111111111112</v>
@@ -2015,15 +2036,15 @@
         <v>0.59375</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D42" s="2">
         <v>0.4284722222222222</v>
@@ -2032,15 +2053,15 @@
         <v>0.57430555555555551</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="B43" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="D43" s="2">
         <v>0.5395833333333333</v>
@@ -2049,91 +2070,132 @@
         <v>0.59583333333333333</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D44" s="2">
         <v>0.4548611111111111</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D45" s="2">
         <v>0.55069444444444449</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D46" s="2">
         <v>0.47222222222222227</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D47" s="2">
         <v>0.60763888888888895</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D48" s="2">
         <v>0.49444444444444446</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D49" s="2">
         <v>0.40972222222222227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B53" t="s">
+        <v>76</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>